<commit_message>
Chirag Chat id added
</commit_message>
<xml_diff>
--- a/permissionIDs.xlsx
+++ b/permissionIDs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,6 +66,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -113,7 +116,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -148,7 +151,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,25 +360,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>468247330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>427374227</v>
       </c>
     </row>
   </sheetData>
@@ -389,7 +397,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -401,7 +409,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Addition of permission id
</commit_message>
<xml_diff>
--- a/permissionIDs.xlsx
+++ b/permissionIDs.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,8 +386,14 @@
         <v>427374227</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>594666386</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Addition of Sid and Shailesh to bot
</commit_message>
<xml_diff>
--- a/permissionIDs.xlsx
+++ b/permissionIDs.xlsx
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,6 +389,16 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>594666386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>521642198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>441895023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added permission for user praveen bajaj
</commit_message>
<xml_diff>
--- a/permissionIDs.xlsx
+++ b/permissionIDs.xlsx
@@ -360,7 +360,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -401,6 +401,11 @@
         <v>441895023</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>552137934</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
removal of permissions from shailesh, praveen
</commit_message>
<xml_diff>
--- a/permissionIDs.xlsx
+++ b/permissionIDs.xlsx
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,21 +391,6 @@
         <v>594666386</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>521642198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>441895023</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>552137934</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding puneet id : 681273062
</commit_message>
<xml_diff>
--- a/permissionIDs.xlsx
+++ b/permissionIDs.xlsx
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,6 +391,11 @@
         <v>594666386</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>681273062</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>